<commit_message>
Revert "Merge pull request #9 from Gesproprac3/1-add-cd-cover-173"
This reverts commit f210373de786974d22defe2f8d2d0f37f84f08d3, reversing
changes made to 0779f0da8c495e512290a5578f9d2ed4ff8393f9.
</commit_message>
<xml_diff>
--- a/docs/rst/anexos/Registro-tiempo.xlsx
+++ b/docs/rst/anexos/Registro-tiempo.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="180" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="155" uniqueCount="26">
   <si>
     <t xml:space="preserve">Story points </t>
   </si>
@@ -102,33 +102,6 @@
   </si>
   <si>
     <t>Sprint 16</t>
-  </si>
-  <si>
-    <t>Sprint 17</t>
-  </si>
-  <si>
-    <t>Sprint 18</t>
-  </si>
-  <si>
-    <t>Bug</t>
-  </si>
-  <si>
-    <t>Issues</t>
-  </si>
-  <si>
-    <t>Tiempo</t>
-  </si>
-  <si>
-    <t>Documentation</t>
-  </si>
-  <si>
-    <t>Feature</t>
-  </si>
-  <si>
-    <t>Research</t>
-  </si>
-  <si>
-    <t>Testing</t>
   </si>
 </sst>
 </file>
@@ -375,7 +348,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="30">
+  <cellXfs count="28">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
@@ -452,477 +425,153 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="266">
-    <dxf>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0">
-        <left/>
-        <right style="medium">
-          <color indexed="64"/>
-        </right>
-        <top/>
-        <bottom/>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left/>
-        <right style="medium">
-          <color indexed="64"/>
-        </right>
-        <top/>
-        <bottom/>
-      </border>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="medium">
-          <color indexed="64"/>
-        </left>
-        <right/>
-        <top/>
-        <bottom/>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left style="medium">
-          <color indexed="64"/>
-        </left>
-        <right/>
-        <top/>
-        <bottom/>
-      </border>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0">
-        <left/>
-        <right style="medium">
-          <color indexed="64"/>
-        </right>
-        <top/>
-        <bottom/>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left/>
-        <right style="medium">
-          <color indexed="64"/>
-        </right>
-        <top/>
-        <bottom/>
-      </border>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="medium">
-          <color indexed="64"/>
-        </left>
-        <right/>
-        <top/>
-        <bottom/>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left style="medium">
-          <color indexed="64"/>
-        </left>
-        <right/>
-        <top/>
-        <bottom/>
-      </border>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0">
-        <left/>
-        <right style="medium">
-          <color indexed="64"/>
-        </right>
-        <top/>
-        <bottom/>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left/>
-        <right style="medium">
-          <color indexed="64"/>
-        </right>
-        <top/>
-        <bottom/>
-      </border>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="medium">
-          <color indexed="64"/>
-        </left>
-        <right/>
-        <top/>
-        <bottom/>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left style="medium">
-          <color indexed="64"/>
-        </left>
-        <right/>
-        <top/>
-        <bottom/>
-      </border>
-    </dxf>
-    <dxf>
-      <border>
-        <bottom style="medium">
-          <color indexed="64"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <border diagonalUp="0" diagonalDown="0">
-        <left/>
-        <right/>
-        <top/>
-        <bottom/>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0">
-        <left/>
-        <right style="medium">
-          <color indexed="64"/>
-        </right>
-        <top/>
-        <bottom/>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left/>
-        <right style="medium">
-          <color indexed="64"/>
-        </right>
-        <top/>
-        <bottom/>
-      </border>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="medium">
-          <color indexed="64"/>
-        </left>
-        <right/>
-        <top/>
-        <bottom/>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left style="medium">
-          <color indexed="64"/>
-        </left>
-        <right/>
-        <top/>
-        <bottom/>
-      </border>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0">
-        <left/>
-        <right style="medium">
-          <color indexed="64"/>
-        </right>
-        <top/>
-        <bottom/>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left/>
-        <right style="medium">
-          <color indexed="64"/>
-        </right>
-        <top/>
-        <bottom/>
-      </border>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="medium">
-          <color indexed="64"/>
-        </left>
-        <right/>
-        <top/>
-        <bottom/>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left style="medium">
-          <color indexed="64"/>
-        </left>
-        <right/>
-        <top/>
-        <bottom/>
-      </border>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0">
-        <left/>
-        <right style="medium">
-          <color indexed="64"/>
-        </right>
-        <top/>
-        <bottom/>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left/>
-        <right style="medium">
-          <color indexed="64"/>
-        </right>
-        <top/>
-        <bottom/>
-      </border>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="medium">
-          <color indexed="64"/>
-        </left>
-        <right/>
-        <top/>
-        <bottom/>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left style="medium">
-          <color indexed="64"/>
-        </left>
-        <right/>
-        <top/>
-        <bottom/>
-      </border>
-    </dxf>
-    <dxf>
-      <border>
-        <bottom style="medium">
-          <color indexed="64"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <border diagonalUp="0" diagonalDown="0">
-        <left/>
-        <right/>
-        <top/>
-        <bottom/>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left/>
-        <right style="medium">
-          <color indexed="64"/>
-        </right>
-        <top/>
-        <bottom/>
-      </border>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0">
-        <left/>
-        <right style="medium">
-          <color indexed="64"/>
-        </right>
-        <top/>
-        <bottom/>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left style="medium">
-          <color indexed="64"/>
-        </left>
-        <right/>
-        <top/>
-        <bottom/>
-      </border>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="medium">
-          <color indexed="64"/>
-        </left>
-        <right/>
-        <top/>
-        <bottom/>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left/>
-        <right style="medium">
-          <color indexed="64"/>
-        </right>
-        <top/>
-        <bottom/>
-      </border>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0">
-        <left/>
-        <right style="medium">
-          <color indexed="64"/>
-        </right>
-        <top/>
-        <bottom/>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left style="medium">
-          <color indexed="64"/>
-        </left>
-        <right/>
-        <top/>
-        <bottom/>
-      </border>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="medium">
-          <color indexed="64"/>
-        </left>
-        <right/>
-        <top/>
-        <bottom/>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left/>
-        <right style="medium">
-          <color indexed="64"/>
-        </right>
-        <top/>
-        <bottom/>
-      </border>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0">
-        <left/>
-        <right style="medium">
-          <color indexed="64"/>
-        </right>
-        <top/>
-        <bottom/>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left style="medium">
-          <color indexed="64"/>
-        </left>
-        <right/>
-        <top/>
-        <bottom/>
-      </border>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="medium">
-          <color indexed="64"/>
-        </left>
-        <right/>
-        <top/>
-        <bottom/>
-        <vertical/>
-        <horizontal/>
+  <dxfs count="238">
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left/>
+        <right style="medium">
+          <color indexed="64"/>
+        </right>
+        <top/>
+        <bottom/>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left/>
+        <right style="medium">
+          <color indexed="64"/>
+        </right>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="medium">
+          <color indexed="64"/>
+        </left>
+        <right/>
+        <top/>
+        <bottom/>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="medium">
+          <color indexed="64"/>
+        </left>
+        <right/>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left/>
+        <right style="medium">
+          <color indexed="64"/>
+        </right>
+        <top/>
+        <bottom/>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left/>
+        <right style="medium">
+          <color indexed="64"/>
+        </right>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="medium">
+          <color indexed="64"/>
+        </left>
+        <right/>
+        <top/>
+        <bottom/>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="medium">
+          <color indexed="64"/>
+        </left>
+        <right/>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left/>
+        <right style="medium">
+          <color indexed="64"/>
+        </right>
+        <top/>
+        <bottom/>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left/>
+        <right style="medium">
+          <color indexed="64"/>
+        </right>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="medium">
+          <color indexed="64"/>
+        </left>
+        <right/>
+        <top/>
+        <bottom/>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="medium">
+          <color indexed="64"/>
+        </left>
+        <right/>
+        <top/>
+        <bottom/>
       </border>
     </dxf>
     <dxf>
@@ -3531,1179 +3180,9 @@
 </styleSheet>
 </file>
 
-<file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
-  <c:date1904 val="0"/>
-  <c:lang val="es-ES"/>
-  <c:roundedCorners val="0"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
-      <c14:style val="102"/>
-    </mc:Choice>
-    <mc:Fallback>
-      <c:style val="2"/>
-    </mc:Fallback>
-  </mc:AlternateContent>
-  <c:chart>
-    <c:title>
-      <c:overlay val="0"/>
-      <c:spPr>
-        <a:noFill/>
-        <a:ln>
-          <a:noFill/>
-        </a:ln>
-        <a:effectLst/>
-      </c:spPr>
-      <c:txPr>
-        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-        <a:lstStyle/>
-        <a:p>
-          <a:pPr>
-            <a:defRPr sz="1400" b="1" i="0" u="none" strike="noStrike" kern="1200" cap="all" spc="50" baseline="0">
-              <a:solidFill>
-                <a:schemeClr val="tx1">
-                  <a:lumMod val="65000"/>
-                  <a:lumOff val="35000"/>
-                </a:schemeClr>
-              </a:solidFill>
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:defRPr>
-          </a:pPr>
-          <a:endParaRPr lang="es-ES"/>
-        </a:p>
-      </c:txPr>
-    </c:title>
-    <c:autoTitleDeleted val="0"/>
-    <c:plotArea>
-      <c:layout/>
-      <c:pieChart>
-        <c:varyColors val="1"/>
-        <c:ser>
-          <c:idx val="0"/>
-          <c:order val="0"/>
-          <c:tx>
-            <c:strRef>
-              <c:f>Hoja1!$B$268:$B$272</c:f>
-              <c:strCache>
-                <c:ptCount val="5"/>
-                <c:pt idx="0">
-                  <c:v>Bug</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>Documentation</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>Feature</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>Research</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>Testing</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:tx>
-          <c:dPt>
-            <c:idx val="0"/>
-            <c:bubble3D val="0"/>
-            <c:spPr>
-              <a:solidFill>
-                <a:schemeClr val="accent1"/>
-              </a:solidFill>
-              <a:ln>
-                <a:noFill/>
-              </a:ln>
-              <a:effectLst/>
-              <a:scene3d>
-                <a:camera prst="orthographicFront"/>
-                <a:lightRig rig="brightRoom" dir="t"/>
-              </a:scene3d>
-              <a:sp3d prstMaterial="flat">
-                <a:bevelT w="50800" h="101600" prst="angle"/>
-                <a:contourClr>
-                  <a:srgbClr val="000000"/>
-                </a:contourClr>
-              </a:sp3d>
-            </c:spPr>
-          </c:dPt>
-          <c:dPt>
-            <c:idx val="1"/>
-            <c:bubble3D val="0"/>
-            <c:spPr>
-              <a:solidFill>
-                <a:schemeClr val="accent2"/>
-              </a:solidFill>
-              <a:ln>
-                <a:noFill/>
-              </a:ln>
-              <a:effectLst/>
-              <a:scene3d>
-                <a:camera prst="orthographicFront"/>
-                <a:lightRig rig="brightRoom" dir="t"/>
-              </a:scene3d>
-              <a:sp3d prstMaterial="flat">
-                <a:bevelT w="50800" h="101600" prst="angle"/>
-                <a:contourClr>
-                  <a:srgbClr val="000000"/>
-                </a:contourClr>
-              </a:sp3d>
-            </c:spPr>
-          </c:dPt>
-          <c:dPt>
-            <c:idx val="2"/>
-            <c:bubble3D val="0"/>
-            <c:spPr>
-              <a:solidFill>
-                <a:schemeClr val="accent3"/>
-              </a:solidFill>
-              <a:ln>
-                <a:noFill/>
-              </a:ln>
-              <a:effectLst/>
-              <a:scene3d>
-                <a:camera prst="orthographicFront"/>
-                <a:lightRig rig="brightRoom" dir="t"/>
-              </a:scene3d>
-              <a:sp3d prstMaterial="flat">
-                <a:bevelT w="50800" h="101600" prst="angle"/>
-                <a:contourClr>
-                  <a:srgbClr val="000000"/>
-                </a:contourClr>
-              </a:sp3d>
-            </c:spPr>
-          </c:dPt>
-          <c:dPt>
-            <c:idx val="3"/>
-            <c:bubble3D val="0"/>
-            <c:spPr>
-              <a:solidFill>
-                <a:schemeClr val="accent4"/>
-              </a:solidFill>
-              <a:ln>
-                <a:noFill/>
-              </a:ln>
-              <a:effectLst/>
-              <a:scene3d>
-                <a:camera prst="orthographicFront"/>
-                <a:lightRig rig="brightRoom" dir="t"/>
-              </a:scene3d>
-              <a:sp3d prstMaterial="flat">
-                <a:bevelT w="50800" h="101600" prst="angle"/>
-                <a:contourClr>
-                  <a:srgbClr val="000000"/>
-                </a:contourClr>
-              </a:sp3d>
-            </c:spPr>
-          </c:dPt>
-          <c:dPt>
-            <c:idx val="4"/>
-            <c:bubble3D val="0"/>
-            <c:spPr>
-              <a:solidFill>
-                <a:schemeClr val="accent5"/>
-              </a:solidFill>
-              <a:ln>
-                <a:noFill/>
-              </a:ln>
-              <a:effectLst/>
-              <a:scene3d>
-                <a:camera prst="orthographicFront"/>
-                <a:lightRig rig="brightRoom" dir="t"/>
-              </a:scene3d>
-              <a:sp3d prstMaterial="flat">
-                <a:bevelT w="50800" h="101600" prst="angle"/>
-                <a:contourClr>
-                  <a:srgbClr val="000000"/>
-                </a:contourClr>
-              </a:sp3d>
-            </c:spPr>
-          </c:dPt>
-          <c:dLbls>
-            <c:spPr>
-              <a:noFill/>
-              <a:ln>
-                <a:noFill/>
-              </a:ln>
-              <a:effectLst/>
-            </c:spPr>
-            <c:txPr>
-              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
-                <a:spAutoFit/>
-              </a:bodyPr>
-              <a:lstStyle/>
-              <a:p>
-                <a:pPr>
-                  <a:defRPr sz="900" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                    <a:solidFill>
-                      <a:schemeClr val="lt1"/>
-                    </a:solidFill>
-                    <a:latin typeface="+mn-lt"/>
-                    <a:ea typeface="+mn-ea"/>
-                    <a:cs typeface="+mn-cs"/>
-                  </a:defRPr>
-                </a:pPr>
-                <a:endParaRPr lang="es-ES"/>
-              </a:p>
-            </c:txPr>
-            <c:dLblPos val="inEnd"/>
-            <c:showLegendKey val="0"/>
-            <c:showVal val="0"/>
-            <c:showCatName val="0"/>
-            <c:showSerName val="0"/>
-            <c:showPercent val="1"/>
-            <c:showBubbleSize val="0"/>
-            <c:showLeaderLines val="1"/>
-            <c:leaderLines>
-              <c:spPr>
-                <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-                  <a:solidFill>
-                    <a:schemeClr val="tx1">
-                      <a:lumMod val="35000"/>
-                      <a:lumOff val="65000"/>
-                    </a:schemeClr>
-                  </a:solidFill>
-                  <a:round/>
-                </a:ln>
-                <a:effectLst/>
-              </c:spPr>
-            </c:leaderLines>
-            <c:extLst>
-              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
-            </c:extLst>
-          </c:dLbls>
-          <c:cat>
-            <c:strRef>
-              <c:f>Hoja1!$B$268:$B$272</c:f>
-              <c:strCache>
-                <c:ptCount val="5"/>
-                <c:pt idx="0">
-                  <c:v>Bug</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>Documentation</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>Feature</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>Research</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>Testing</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:cat>
-          <c:val>
-            <c:numRef>
-              <c:f>Hoja1!$L$268:$L$272</c:f>
-              <c:numCache>
-                <c:formatCode>0.00%</c:formatCode>
-                <c:ptCount val="5"/>
-                <c:pt idx="0">
-                  <c:v>5.1322418136020148E-2</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>0.20906801007556675</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>0.51668765743073053</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>0.16120906801007556</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>6.1712846347607056E-2</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:val>
-          <c:extLst>
-            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000000-04FC-42D0-BE7C-F4A654DE0DA0}"/>
-            </c:ext>
-          </c:extLst>
-        </c:ser>
-        <c:dLbls>
-          <c:dLblPos val="inEnd"/>
-          <c:showLegendKey val="0"/>
-          <c:showVal val="0"/>
-          <c:showCatName val="0"/>
-          <c:showSerName val="0"/>
-          <c:showPercent val="1"/>
-          <c:showBubbleSize val="0"/>
-          <c:showLeaderLines val="1"/>
-        </c:dLbls>
-        <c:firstSliceAng val="0"/>
-      </c:pieChart>
-      <c:spPr>
-        <a:noFill/>
-        <a:ln>
-          <a:noFill/>
-        </a:ln>
-        <a:effectLst/>
-      </c:spPr>
-    </c:plotArea>
-    <c:legend>
-      <c:legendPos val="t"/>
-      <c:overlay val="0"/>
-      <c:spPr>
-        <a:noFill/>
-        <a:ln>
-          <a:noFill/>
-        </a:ln>
-        <a:effectLst/>
-      </c:spPr>
-      <c:txPr>
-        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-        <a:lstStyle/>
-        <a:p>
-          <a:pPr rtl="0">
-            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-              <a:solidFill>
-                <a:schemeClr val="tx1">
-                  <a:lumMod val="65000"/>
-                  <a:lumOff val="35000"/>
-                </a:schemeClr>
-              </a:solidFill>
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:defRPr>
-          </a:pPr>
-          <a:endParaRPr lang="es-ES"/>
-        </a:p>
-      </c:txPr>
-    </c:legend>
-    <c:plotVisOnly val="1"/>
-    <c:dispBlanksAs val="gap"/>
-    <c:showDLblsOverMax val="0"/>
-  </c:chart>
-  <c:spPr>
-    <a:solidFill>
-      <a:schemeClr val="bg1"/>
-    </a:solidFill>
-    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-      <a:solidFill>
-        <a:schemeClr val="tx1">
-          <a:lumMod val="15000"/>
-          <a:lumOff val="85000"/>
-        </a:schemeClr>
-      </a:solidFill>
-      <a:round/>
-    </a:ln>
-    <a:effectLst/>
-  </c:spPr>
-  <c:txPr>
-    <a:bodyPr/>
-    <a:lstStyle/>
-    <a:p>
-      <a:pPr>
-        <a:defRPr/>
-      </a:pPr>
-      <a:endParaRPr lang="es-ES"/>
-    </a:p>
-  </c:txPr>
-  <c:printSettings>
-    <c:headerFooter/>
-    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
-    <c:pageSetup/>
-  </c:printSettings>
-</c:chartSpace>
-</file>
-
-<file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
-<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
-  <a:schemeClr val="accent1"/>
-  <a:schemeClr val="accent2"/>
-  <a:schemeClr val="accent3"/>
-  <a:schemeClr val="accent4"/>
-  <a:schemeClr val="accent5"/>
-  <a:schemeClr val="accent6"/>
-  <cs:variation/>
-  <cs:variation>
-    <a:lumMod val="60000"/>
-  </cs:variation>
-  <cs:variation>
-    <a:lumMod val="80000"/>
-    <a:lumOff val="20000"/>
-  </cs:variation>
-  <cs:variation>
-    <a:lumMod val="80000"/>
-  </cs:variation>
-  <cs:variation>
-    <a:lumMod val="60000"/>
-    <a:lumOff val="40000"/>
-  </cs:variation>
-  <cs:variation>
-    <a:lumMod val="50000"/>
-  </cs:variation>
-  <cs:variation>
-    <a:lumMod val="70000"/>
-    <a:lumOff val="30000"/>
-  </cs:variation>
-  <cs:variation>
-    <a:lumMod val="70000"/>
-  </cs:variation>
-  <cs:variation>
-    <a:lumMod val="50000"/>
-    <a:lumOff val="50000"/>
-  </cs:variation>
-</cs:colorStyle>
-</file>
-
-<file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
-<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="258">
-  <cs:axisTitle>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:axisTitle>
-  <cs:categoryAxis>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:categoryAxis>
-  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:solidFill>
-        <a:schemeClr val="bg1"/>
-      </a:solidFill>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="15000"/>
-            <a:lumOff val="85000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:chartArea>
-  <cs:dataLabel>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="lt1"/>
-    </cs:fontRef>
-    <cs:defRPr sz="900" b="1" kern="1200"/>
-  </cs:dataLabel>
-  <cs:dataLabelCallout>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:solidFill>
-        <a:schemeClr val="lt1"/>
-      </a:solidFill>
-      <a:ln>
-        <a:solidFill>
-          <a:schemeClr val="dk1">
-            <a:lumMod val="25000"/>
-            <a:lumOff val="75000"/>
-          </a:schemeClr>
-        </a:solidFill>
-      </a:ln>
-    </cs:spPr>
-    <cs:defRPr sz="900" kern="1200"/>
-    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
-      <a:spAutoFit/>
-    </cs:bodyPr>
-  </cs:dataLabelCallout>
-  <cs:dataPoint>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0">
-      <cs:styleClr val="auto"/>
-    </cs:fillRef>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:solidFill>
-        <a:schemeClr val="phClr"/>
-      </a:solidFill>
-      <a:scene3d>
-        <a:camera prst="orthographicFront"/>
-        <a:lightRig rig="brightRoom" dir="t"/>
-      </a:scene3d>
-      <a:sp3d prstMaterial="flat">
-        <a:bevelT w="50800" h="101600" prst="angle"/>
-        <a:contourClr>
-          <a:srgbClr val="000000"/>
-        </a:contourClr>
-      </a:sp3d>
-    </cs:spPr>
-  </cs:dataPoint>
-  <cs:dataPoint3D>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0">
-      <cs:styleClr val="auto"/>
-    </cs:fillRef>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:solidFill>
-        <a:schemeClr val="phClr"/>
-      </a:solidFill>
-      <a:ln w="19050">
-        <a:solidFill>
-          <a:schemeClr val="lt1"/>
-        </a:solidFill>
-      </a:ln>
-    </cs:spPr>
-  </cs:dataPoint3D>
-  <cs:dataPointLine>
-    <cs:lnRef idx="0">
-      <cs:styleClr val="auto"/>
-    </cs:lnRef>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="28575" cap="rnd">
-        <a:solidFill>
-          <a:schemeClr val="phClr"/>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:dataPointLine>
-  <cs:dataPointMarker>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0">
-      <cs:styleClr val="auto"/>
-    </cs:fillRef>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:solidFill>
-        <a:schemeClr val="phClr"/>
-      </a:solidFill>
-      <a:ln w="9525">
-        <a:solidFill>
-          <a:schemeClr val="lt1"/>
-        </a:solidFill>
-      </a:ln>
-    </cs:spPr>
-  </cs:dataPointMarker>
-  <cs:dataPointMarkerLayout symbol="circle" size="6"/>
-  <cs:dataPointWireframe>
-    <cs:lnRef idx="0">
-      <cs:styleClr val="auto"/>
-    </cs:lnRef>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="rnd">
-        <a:solidFill>
-          <a:schemeClr val="phClr"/>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:dataPointWireframe>
-  <cs:dataTable>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:noFill/>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="15000"/>
-            <a:lumOff val="85000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:dataTable>
-  <cs:downBar>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:solidFill>
-        <a:schemeClr val="dk1">
-          <a:lumMod val="75000"/>
-          <a:lumOff val="25000"/>
-        </a:schemeClr>
-      </a:solidFill>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="65000"/>
-            <a:lumOff val="35000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:downBar>
-  <cs:dropLine>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="35000"/>
-            <a:lumOff val="65000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:dropLine>
-  <cs:errorBar>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="65000"/>
-            <a:lumOff val="35000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:errorBar>
-  <cs:floor>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:noFill/>
-      <a:ln>
-        <a:noFill/>
-      </a:ln>
-    </cs:spPr>
-  </cs:floor>
-  <cs:gridlineMajor>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="15000"/>
-            <a:lumOff val="85000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:gridlineMajor>
-  <cs:gridlineMinor>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="5000"/>
-            <a:lumOff val="95000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:gridlineMinor>
-  <cs:hiLoLine>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="50000"/>
-            <a:lumOff val="50000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:hiLoLine>
-  <cs:leaderLine>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="35000"/>
-            <a:lumOff val="65000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:leaderLine>
-  <cs:legend>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:legend>
-  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-  </cs:plotArea>
-  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-  </cs:plotArea3D>
-  <cs:seriesAxis>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:seriesAxis>
-  <cs:seriesLine>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="35000"/>
-            <a:lumOff val="65000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:seriesLine>
-  <cs:title>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:defRPr sz="1400" b="1" i="0" kern="1200" cap="all" spc="50" baseline="0"/>
-  </cs:title>
-  <cs:trendline>
-    <cs:lnRef idx="0">
-      <cs:styleClr val="auto"/>
-    </cs:lnRef>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="19050" cap="rnd">
-        <a:solidFill>
-          <a:schemeClr val="phClr"/>
-        </a:solidFill>
-        <a:prstDash val="sysDash"/>
-      </a:ln>
-    </cs:spPr>
-  </cs:trendline>
-  <cs:trendlineLabel>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:trendlineLabel>
-  <cs:upBar>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:solidFill>
-        <a:schemeClr val="lt1"/>
-      </a:solidFill>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="65000"/>
-            <a:lumOff val="35000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:upBar>
-  <cs:valueAxis>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:valueAxis>
-  <cs:wall>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:noFill/>
-      <a:ln>
-        <a:noFill/>
-      </a:ln>
-    </cs:spPr>
-  </cs:wall>
-</cs:chartStyle>
-</file>
-
-<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>4</xdr:col>
-      <xdr:colOff>348533</xdr:colOff>
-      <xdr:row>274</xdr:row>
-      <xdr:rowOff>31648</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>9</xdr:col>
-      <xdr:colOff>515886</xdr:colOff>
-      <xdr:row>288</xdr:row>
-      <xdr:rowOff>111945</xdr:rowOff>
-    </xdr:to>
-    <xdr:graphicFrame macro="">
-      <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="2" name="Gráfico 1"/>
-        <xdr:cNvGraphicFramePr/>
-      </xdr:nvGraphicFramePr>
-      <xdr:xfrm>
-        <a:off x="0" y="0"/>
-        <a:ext cx="0" cy="0"/>
-      </xdr:xfrm>
-      <a:graphic>
-        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
-          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
-        </a:graphicData>
-      </a:graphic>
-    </xdr:graphicFrame>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-</xdr:wsDr>
-</file>
-
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="7" name="Tabla18" displayName="Tabla18" ref="B17:G26" headerRowDxfId="265" headerRowBorderDxfId="264">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="7" name="Tabla18" displayName="Tabla18" ref="B17:G26" headerRowDxfId="237" headerRowBorderDxfId="236">
   <autoFilter ref="B17:G26">
-    <filterColumn colId="0" hiddenButton="1"/>
-    <filterColumn colId="1" hiddenButton="1"/>
-    <filterColumn colId="2" hiddenButton="1"/>
-    <filterColumn colId="3" hiddenButton="1"/>
-    <filterColumn colId="4" hiddenButton="1"/>
-    <filterColumn colId="5" hiddenButton="1"/>
-  </autoFilter>
-  <tableColumns count="6">
-    <tableColumn id="1" name="Story points " totalsRowLabel="Total" dataDxfId="263" totalsRowDxfId="262"/>
-    <tableColumn id="2" name="Min." dataDxfId="261" totalsRowDxfId="260"/>
-    <tableColumn id="3" name="Estimado" dataDxfId="259" totalsRowDxfId="258"/>
-    <tableColumn id="4" name="Total" dataDxfId="257" totalsRowDxfId="256"/>
-    <tableColumn id="5" name="Real" dataDxfId="255" totalsRowDxfId="254"/>
-    <tableColumn id="6" name="Total3" totalsRowFunction="sum" dataDxfId="253" totalsRowDxfId="252"/>
-  </tableColumns>
-  <tableStyleInfo name="TableStyleMedium16" showFirstColumn="0" showLastColumn="0" showRowStripes="0" showColumnStripes="1"/>
-</table>
-</file>
-
-<file path=xl/tables/table10.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="6" name="Tabla181011234567" displayName="Tabla181011234567" ref="B129:G138" headerRowDxfId="139" headerRowBorderDxfId="138">
-  <autoFilter ref="B129:G138"/>
-  <tableColumns count="6">
-    <tableColumn id="1" name="Story points " totalsRowLabel="Total" dataDxfId="137" totalsRowDxfId="136"/>
-    <tableColumn id="2" name="Min." dataDxfId="135" totalsRowDxfId="134"/>
-    <tableColumn id="3" name="Estimado" dataDxfId="133" totalsRowDxfId="132"/>
-    <tableColumn id="4" name="Total" dataDxfId="131" totalsRowDxfId="130"/>
-    <tableColumn id="5" name="Real" dataDxfId="129" totalsRowDxfId="128"/>
-    <tableColumn id="6" name="Total3" totalsRowFunction="sum" dataDxfId="127" totalsRowDxfId="126"/>
-  </tableColumns>
-  <tableStyleInfo name="TableStyleMedium16" showFirstColumn="0" showLastColumn="0" showRowStripes="0" showColumnStripes="1"/>
-</table>
-</file>
-
-<file path=xl/tables/table11.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="11" name="Tabla18101123456712" displayName="Tabla18101123456712" ref="B143:G152" headerRowDxfId="125" headerRowBorderDxfId="124">
-  <autoFilter ref="B143:G152"/>
-  <tableColumns count="6">
-    <tableColumn id="1" name="Story points " totalsRowLabel="Total" dataDxfId="123" totalsRowDxfId="122"/>
-    <tableColumn id="2" name="Min." dataDxfId="121" totalsRowDxfId="120"/>
-    <tableColumn id="3" name="Estimado" dataDxfId="119" totalsRowDxfId="118"/>
-    <tableColumn id="4" name="Total" dataDxfId="117" totalsRowDxfId="116"/>
-    <tableColumn id="5" name="Real" dataDxfId="115" totalsRowDxfId="114"/>
-    <tableColumn id="6" name="Total3" totalsRowFunction="sum" dataDxfId="113" totalsRowDxfId="112"/>
-  </tableColumns>
-  <tableStyleInfo name="TableStyleMedium16" showFirstColumn="0" showLastColumn="0" showRowStripes="0" showColumnStripes="1"/>
-</table>
-</file>
-
-<file path=xl/tables/table12.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="12" name="Tabla1810112345671213" displayName="Tabla1810112345671213" ref="B157:G166" headerRowDxfId="111" headerRowBorderDxfId="110">
-  <autoFilter ref="B157:G166"/>
-  <tableColumns count="6">
-    <tableColumn id="1" name="Story points " totalsRowLabel="Total" dataDxfId="109" totalsRowDxfId="108"/>
-    <tableColumn id="2" name="Min." dataDxfId="107" totalsRowDxfId="106"/>
-    <tableColumn id="3" name="Estimado" dataDxfId="105" totalsRowDxfId="104"/>
-    <tableColumn id="4" name="Total" dataDxfId="103" totalsRowDxfId="102"/>
-    <tableColumn id="5" name="Real" dataDxfId="101" totalsRowDxfId="100"/>
-    <tableColumn id="6" name="Total3" totalsRowFunction="sum" dataDxfId="99" totalsRowDxfId="98"/>
-  </tableColumns>
-  <tableStyleInfo name="TableStyleMedium16" showFirstColumn="0" showLastColumn="0" showRowStripes="0" showColumnStripes="1"/>
-</table>
-</file>
-
-<file path=xl/tables/table13.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="13" name="Tabla181011234567121314" displayName="Tabla181011234567121314" ref="B171:G180" headerRowDxfId="97" headerRowBorderDxfId="96">
-  <autoFilter ref="B171:G180"/>
-  <tableColumns count="6">
-    <tableColumn id="1" name="Story points " totalsRowLabel="Total" dataDxfId="95" totalsRowDxfId="94"/>
-    <tableColumn id="2" name="Min." dataDxfId="93" totalsRowDxfId="92"/>
-    <tableColumn id="3" name="Estimado" dataDxfId="91" totalsRowDxfId="90"/>
-    <tableColumn id="4" name="Total" dataDxfId="89" totalsRowDxfId="88"/>
-    <tableColumn id="5" name="Real" dataDxfId="87" totalsRowDxfId="86"/>
-    <tableColumn id="6" name="Total3" totalsRowFunction="sum" dataDxfId="85" totalsRowDxfId="84"/>
-  </tableColumns>
-  <tableStyleInfo name="TableStyleMedium16" showFirstColumn="0" showLastColumn="0" showRowStripes="0" showColumnStripes="1"/>
-</table>
-</file>
-
-<file path=xl/tables/table14.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="14" name="Tabla18101123456712131415" displayName="Tabla18101123456712131415" ref="B185:G194" headerRowDxfId="83" headerRowBorderDxfId="82">
-  <autoFilter ref="B185:G194"/>
-  <tableColumns count="6">
-    <tableColumn id="1" name="Story points " totalsRowLabel="Total" dataDxfId="81" totalsRowDxfId="80"/>
-    <tableColumn id="2" name="Min." dataDxfId="79" totalsRowDxfId="78"/>
-    <tableColumn id="3" name="Estimado" dataDxfId="77" totalsRowDxfId="76"/>
-    <tableColumn id="4" name="Total" dataDxfId="75" totalsRowDxfId="74"/>
-    <tableColumn id="5" name="Real" dataDxfId="73" totalsRowDxfId="72"/>
-    <tableColumn id="6" name="Total3" totalsRowFunction="sum" dataDxfId="71" totalsRowDxfId="70"/>
-  </tableColumns>
-  <tableStyleInfo name="TableStyleMedium16" showFirstColumn="0" showLastColumn="0" showRowStripes="0" showColumnStripes="1"/>
-</table>
-</file>
-
-<file path=xl/tables/table15.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="15" name="Tabla1810112345671213141516" displayName="Tabla1810112345671213141516" ref="B199:G208" headerRowDxfId="69" headerRowBorderDxfId="68">
-  <autoFilter ref="B199:G208"/>
-  <tableColumns count="6">
-    <tableColumn id="1" name="Story points " totalsRowLabel="Total" dataDxfId="67" totalsRowDxfId="66"/>
-    <tableColumn id="2" name="Min." dataDxfId="65" totalsRowDxfId="64"/>
-    <tableColumn id="3" name="Estimado" dataDxfId="63" totalsRowDxfId="62"/>
-    <tableColumn id="4" name="Total" dataDxfId="61" totalsRowDxfId="60"/>
-    <tableColumn id="5" name="Real" dataDxfId="59" totalsRowDxfId="58"/>
-    <tableColumn id="6" name="Total3" totalsRowFunction="sum" dataDxfId="57" totalsRowDxfId="56"/>
-  </tableColumns>
-  <tableStyleInfo name="TableStyleMedium16" showFirstColumn="0" showLastColumn="0" showRowStripes="0" showColumnStripes="1"/>
-</table>
-</file>
-
-<file path=xl/tables/table16.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="16" name="Tabla181011234567121314151617" displayName="Tabla181011234567121314151617" ref="B213:G222" headerRowDxfId="55" headerRowBorderDxfId="54">
-  <autoFilter ref="B213:G222"/>
-  <tableColumns count="6">
-    <tableColumn id="1" name="Story points " totalsRowLabel="Total" dataDxfId="53" totalsRowDxfId="52"/>
-    <tableColumn id="2" name="Min." dataDxfId="51" totalsRowDxfId="50"/>
-    <tableColumn id="3" name="Estimado" dataDxfId="49" totalsRowDxfId="48"/>
-    <tableColumn id="4" name="Total" dataDxfId="47" totalsRowDxfId="46"/>
-    <tableColumn id="5" name="Real" dataDxfId="45" totalsRowDxfId="44"/>
-    <tableColumn id="6" name="Total3" totalsRowFunction="sum" dataDxfId="43" totalsRowDxfId="42"/>
-  </tableColumns>
-  <tableStyleInfo name="TableStyleMedium16" showFirstColumn="0" showLastColumn="0" showRowStripes="0" showColumnStripes="1"/>
-</table>
-</file>
-
-<file path=xl/tables/table17.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="17" name="Tabla18101123456712131415161718" displayName="Tabla18101123456712131415161718" ref="B227:G236" headerRowDxfId="41" headerRowBorderDxfId="40">
-  <autoFilter ref="B227:G236"/>
-  <tableColumns count="6">
-    <tableColumn id="1" name="Story points " totalsRowLabel="Total" dataDxfId="39" totalsRowDxfId="38"/>
-    <tableColumn id="2" name="Min." dataDxfId="37" totalsRowDxfId="36"/>
-    <tableColumn id="3" name="Estimado" dataDxfId="35" totalsRowDxfId="34"/>
-    <tableColumn id="4" name="Total" dataDxfId="33" totalsRowDxfId="32"/>
-    <tableColumn id="5" name="Real" dataDxfId="31" totalsRowDxfId="30"/>
-    <tableColumn id="6" name="Total3" totalsRowFunction="sum" dataDxfId="29" totalsRowDxfId="28"/>
-  </tableColumns>
-  <tableStyleInfo name="TableStyleMedium16" showFirstColumn="0" showLastColumn="0" showRowStripes="0" showColumnStripes="1"/>
-</table>
-</file>
-
-<file path=xl/tables/table18.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="18" name="Tabla1810112345671213141516171819" displayName="Tabla1810112345671213141516171819" ref="B241:G250" headerRowDxfId="27" headerRowBorderDxfId="26">
-  <autoFilter ref="B241:G250"/>
-  <tableColumns count="6">
-    <tableColumn id="1" name="Story points " totalsRowLabel="Total" dataDxfId="24" totalsRowDxfId="25"/>
-    <tableColumn id="2" name="Min." dataDxfId="22" totalsRowDxfId="23"/>
-    <tableColumn id="3" name="Estimado" dataDxfId="20" totalsRowDxfId="21"/>
-    <tableColumn id="4" name="Total" dataDxfId="18" totalsRowDxfId="19"/>
-    <tableColumn id="5" name="Real" dataDxfId="16" totalsRowDxfId="17"/>
-    <tableColumn id="6" name="Total3" totalsRowFunction="sum" dataDxfId="14" totalsRowDxfId="15"/>
-  </tableColumns>
-  <tableStyleInfo name="TableStyleMedium16" showFirstColumn="0" showLastColumn="0" showRowStripes="0" showColumnStripes="1"/>
-</table>
-</file>
-
-<file path=xl/tables/table19.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="19" name="Tabla181011234567121314151617181920" displayName="Tabla181011234567121314151617181920" ref="B255:G264" headerRowDxfId="13" headerRowBorderDxfId="12">
-  <autoFilter ref="B255:G264"/>
-  <tableColumns count="6">
-    <tableColumn id="1" name="Story points " totalsRowLabel="Total" dataDxfId="10" totalsRowDxfId="11"/>
-    <tableColumn id="2" name="Min." dataDxfId="8" totalsRowDxfId="9"/>
-    <tableColumn id="3" name="Estimado" dataDxfId="6" totalsRowDxfId="7"/>
-    <tableColumn id="4" name="Total" dataDxfId="4" totalsRowDxfId="5"/>
-    <tableColumn id="5" name="Real" dataDxfId="2" totalsRowDxfId="3"/>
-    <tableColumn id="6" name="Total3" totalsRowFunction="sum" dataDxfId="0" totalsRowDxfId="1"/>
-  </tableColumns>
-  <tableStyleInfo name="TableStyleMedium16" showFirstColumn="0" showLastColumn="0" showRowStripes="0" showColumnStripes="1"/>
-</table>
-</file>
-
-<file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="8" name="Tabla189" displayName="Tabla189" ref="B3:G12" headerRowDxfId="251" headerRowBorderDxfId="250">
-  <autoFilter ref="B3:G12">
-    <filterColumn colId="0" hiddenButton="1"/>
-    <filterColumn colId="1" hiddenButton="1"/>
-    <filterColumn colId="2" hiddenButton="1"/>
-    <filterColumn colId="3" hiddenButton="1"/>
-    <filterColumn colId="4" hiddenButton="1"/>
-    <filterColumn colId="5" hiddenButton="1"/>
-  </autoFilter>
-  <tableColumns count="6">
-    <tableColumn id="1" name="Story points " totalsRowLabel="Total" dataDxfId="249" totalsRowDxfId="248"/>
-    <tableColumn id="2" name="Min." dataDxfId="247" totalsRowDxfId="246"/>
-    <tableColumn id="3" name="Estimado" dataDxfId="245" totalsRowDxfId="244"/>
-    <tableColumn id="4" name="Total" dataDxfId="243" totalsRowDxfId="242"/>
-    <tableColumn id="5" name="Real" dataDxfId="241" totalsRowDxfId="240"/>
-    <tableColumn id="6" name="Total3" totalsRowFunction="sum" dataDxfId="239" totalsRowDxfId="238"/>
-  </tableColumns>
-  <tableStyleInfo name="TableStyleMedium16" showFirstColumn="0" showLastColumn="0" showRowStripes="0" showColumnStripes="1"/>
-</table>
-</file>
-
-<file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="9" name="Tabla1810" displayName="Tabla1810" ref="B31:G40" headerRowDxfId="237" headerRowBorderDxfId="236">
-  <autoFilter ref="B31:G40">
     <filterColumn colId="0" hiddenButton="1"/>
     <filterColumn colId="1" hiddenButton="1"/>
     <filterColumn colId="2" hiddenButton="1"/>
@@ -4723,9 +3202,129 @@
 </table>
 </file>
 
-<file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="10" name="Tabla181011" displayName="Tabla181011" ref="B45:G54" headerRowDxfId="223" headerRowBorderDxfId="222">
-  <autoFilter ref="B45:G54">
+<file path=xl/tables/table10.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="6" name="Tabla181011234567" displayName="Tabla181011234567" ref="B129:G138" headerRowDxfId="111" headerRowBorderDxfId="110">
+  <autoFilter ref="B129:G138"/>
+  <tableColumns count="6">
+    <tableColumn id="1" name="Story points " totalsRowLabel="Total" dataDxfId="109" totalsRowDxfId="108"/>
+    <tableColumn id="2" name="Min." dataDxfId="107" totalsRowDxfId="106"/>
+    <tableColumn id="3" name="Estimado" dataDxfId="105" totalsRowDxfId="104"/>
+    <tableColumn id="4" name="Total" dataDxfId="103" totalsRowDxfId="102"/>
+    <tableColumn id="5" name="Real" dataDxfId="101" totalsRowDxfId="100"/>
+    <tableColumn id="6" name="Total3" totalsRowFunction="sum" dataDxfId="99" totalsRowDxfId="98"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium16" showFirstColumn="0" showLastColumn="0" showRowStripes="0" showColumnStripes="1"/>
+</table>
+</file>
+
+<file path=xl/tables/table11.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="11" name="Tabla18101123456712" displayName="Tabla18101123456712" ref="B143:G152" headerRowDxfId="97" headerRowBorderDxfId="96">
+  <autoFilter ref="B143:G152"/>
+  <tableColumns count="6">
+    <tableColumn id="1" name="Story points " totalsRowLabel="Total" dataDxfId="95" totalsRowDxfId="94"/>
+    <tableColumn id="2" name="Min." dataDxfId="93" totalsRowDxfId="92"/>
+    <tableColumn id="3" name="Estimado" dataDxfId="91" totalsRowDxfId="90"/>
+    <tableColumn id="4" name="Total" dataDxfId="89" totalsRowDxfId="88"/>
+    <tableColumn id="5" name="Real" dataDxfId="87" totalsRowDxfId="86"/>
+    <tableColumn id="6" name="Total3" totalsRowFunction="sum" dataDxfId="85" totalsRowDxfId="84"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium16" showFirstColumn="0" showLastColumn="0" showRowStripes="0" showColumnStripes="1"/>
+</table>
+</file>
+
+<file path=xl/tables/table12.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="12" name="Tabla1810112345671213" displayName="Tabla1810112345671213" ref="B157:G166" headerRowDxfId="83" headerRowBorderDxfId="82">
+  <autoFilter ref="B157:G166"/>
+  <tableColumns count="6">
+    <tableColumn id="1" name="Story points " totalsRowLabel="Total" dataDxfId="81" totalsRowDxfId="80"/>
+    <tableColumn id="2" name="Min." dataDxfId="79" totalsRowDxfId="78"/>
+    <tableColumn id="3" name="Estimado" dataDxfId="77" totalsRowDxfId="76"/>
+    <tableColumn id="4" name="Total" dataDxfId="75" totalsRowDxfId="74"/>
+    <tableColumn id="5" name="Real" dataDxfId="73" totalsRowDxfId="72"/>
+    <tableColumn id="6" name="Total3" totalsRowFunction="sum" dataDxfId="71" totalsRowDxfId="70"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium16" showFirstColumn="0" showLastColumn="0" showRowStripes="0" showColumnStripes="1"/>
+</table>
+</file>
+
+<file path=xl/tables/table13.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="13" name="Tabla181011234567121314" displayName="Tabla181011234567121314" ref="B171:G180" headerRowDxfId="69" headerRowBorderDxfId="68">
+  <autoFilter ref="B171:G180"/>
+  <tableColumns count="6">
+    <tableColumn id="1" name="Story points " totalsRowLabel="Total" dataDxfId="67" totalsRowDxfId="66"/>
+    <tableColumn id="2" name="Min." dataDxfId="65" totalsRowDxfId="64"/>
+    <tableColumn id="3" name="Estimado" dataDxfId="63" totalsRowDxfId="62"/>
+    <tableColumn id="4" name="Total" dataDxfId="61" totalsRowDxfId="60"/>
+    <tableColumn id="5" name="Real" dataDxfId="59" totalsRowDxfId="58"/>
+    <tableColumn id="6" name="Total3" totalsRowFunction="sum" dataDxfId="57" totalsRowDxfId="56"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium16" showFirstColumn="0" showLastColumn="0" showRowStripes="0" showColumnStripes="1"/>
+</table>
+</file>
+
+<file path=xl/tables/table14.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="14" name="Tabla18101123456712131415" displayName="Tabla18101123456712131415" ref="B185:G194" headerRowDxfId="55" headerRowBorderDxfId="54">
+  <autoFilter ref="B185:G194"/>
+  <tableColumns count="6">
+    <tableColumn id="1" name="Story points " totalsRowLabel="Total" dataDxfId="53" totalsRowDxfId="52"/>
+    <tableColumn id="2" name="Min." dataDxfId="51" totalsRowDxfId="50"/>
+    <tableColumn id="3" name="Estimado" dataDxfId="49" totalsRowDxfId="48"/>
+    <tableColumn id="4" name="Total" dataDxfId="47" totalsRowDxfId="46"/>
+    <tableColumn id="5" name="Real" dataDxfId="45" totalsRowDxfId="44"/>
+    <tableColumn id="6" name="Total3" totalsRowFunction="sum" dataDxfId="43" totalsRowDxfId="42"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium16" showFirstColumn="0" showLastColumn="0" showRowStripes="0" showColumnStripes="1"/>
+</table>
+</file>
+
+<file path=xl/tables/table15.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="15" name="Tabla1810112345671213141516" displayName="Tabla1810112345671213141516" ref="B199:G208" headerRowDxfId="41" headerRowBorderDxfId="40">
+  <autoFilter ref="B199:G208"/>
+  <tableColumns count="6">
+    <tableColumn id="1" name="Story points " totalsRowLabel="Total" dataDxfId="39" totalsRowDxfId="38"/>
+    <tableColumn id="2" name="Min." dataDxfId="37" totalsRowDxfId="36"/>
+    <tableColumn id="3" name="Estimado" dataDxfId="35" totalsRowDxfId="34"/>
+    <tableColumn id="4" name="Total" dataDxfId="33" totalsRowDxfId="32"/>
+    <tableColumn id="5" name="Real" dataDxfId="31" totalsRowDxfId="30"/>
+    <tableColumn id="6" name="Total3" totalsRowFunction="sum" dataDxfId="29" totalsRowDxfId="28"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium16" showFirstColumn="0" showLastColumn="0" showRowStripes="0" showColumnStripes="1"/>
+</table>
+</file>
+
+<file path=xl/tables/table16.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="16" name="Tabla181011234567121314151617" displayName="Tabla181011234567121314151617" ref="B213:G222" headerRowDxfId="27" headerRowBorderDxfId="26">
+  <autoFilter ref="B213:G222"/>
+  <tableColumns count="6">
+    <tableColumn id="1" name="Story points " totalsRowLabel="Total" dataDxfId="25" totalsRowDxfId="24"/>
+    <tableColumn id="2" name="Min." dataDxfId="23" totalsRowDxfId="22"/>
+    <tableColumn id="3" name="Estimado" dataDxfId="21" totalsRowDxfId="20"/>
+    <tableColumn id="4" name="Total" dataDxfId="19" totalsRowDxfId="18"/>
+    <tableColumn id="5" name="Real" dataDxfId="17" totalsRowDxfId="16"/>
+    <tableColumn id="6" name="Total3" totalsRowFunction="sum" dataDxfId="15" totalsRowDxfId="14"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium16" showFirstColumn="0" showLastColumn="0" showRowStripes="0" showColumnStripes="1"/>
+</table>
+</file>
+
+<file path=xl/tables/table17.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="17" name="Tabla18101123456712131415161718" displayName="Tabla18101123456712131415161718" ref="B227:G236" headerRowDxfId="13" headerRowBorderDxfId="12">
+  <autoFilter ref="B227:G236"/>
+  <tableColumns count="6">
+    <tableColumn id="1" name="Story points " totalsRowLabel="Total" dataDxfId="10" totalsRowDxfId="11"/>
+    <tableColumn id="2" name="Min." dataDxfId="8" totalsRowDxfId="9"/>
+    <tableColumn id="3" name="Estimado" dataDxfId="6" totalsRowDxfId="7"/>
+    <tableColumn id="4" name="Total" dataDxfId="4" totalsRowDxfId="5"/>
+    <tableColumn id="5" name="Real" dataDxfId="2" totalsRowDxfId="3"/>
+    <tableColumn id="6" name="Total3" totalsRowFunction="sum" dataDxfId="0" totalsRowDxfId="1"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium16" showFirstColumn="0" showLastColumn="0" showRowStripes="0" showColumnStripes="1"/>
+</table>
+</file>
+
+<file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="8" name="Tabla189" displayName="Tabla189" ref="B3:G12" headerRowDxfId="223" headerRowBorderDxfId="222">
+  <autoFilter ref="B3:G12">
     <filterColumn colId="0" hiddenButton="1"/>
     <filterColumn colId="1" hiddenButton="1"/>
     <filterColumn colId="2" hiddenButton="1"/>
@@ -4745,9 +3344,16 @@
 </table>
 </file>
 
-<file path=xl/tables/table5.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Tabla1810112" displayName="Tabla1810112" ref="B59:G68" headerRowDxfId="209" headerRowBorderDxfId="208">
-  <autoFilter ref="B59:G68"/>
+<file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="9" name="Tabla1810" displayName="Tabla1810" ref="B31:G40" headerRowDxfId="209" headerRowBorderDxfId="208">
+  <autoFilter ref="B31:G40">
+    <filterColumn colId="0" hiddenButton="1"/>
+    <filterColumn colId="1" hiddenButton="1"/>
+    <filterColumn colId="2" hiddenButton="1"/>
+    <filterColumn colId="3" hiddenButton="1"/>
+    <filterColumn colId="4" hiddenButton="1"/>
+    <filterColumn colId="5" hiddenButton="1"/>
+  </autoFilter>
   <tableColumns count="6">
     <tableColumn id="1" name="Story points " totalsRowLabel="Total" dataDxfId="207" totalsRowDxfId="206"/>
     <tableColumn id="2" name="Min." dataDxfId="205" totalsRowDxfId="204"/>
@@ -4760,9 +3366,16 @@
 </table>
 </file>
 
-<file path=xl/tables/table6.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Tabla18101123" displayName="Tabla18101123" ref="B73:G82" headerRowDxfId="195" headerRowBorderDxfId="194">
-  <autoFilter ref="B73:G82"/>
+<file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="10" name="Tabla181011" displayName="Tabla181011" ref="B45:G54" headerRowDxfId="195" headerRowBorderDxfId="194">
+  <autoFilter ref="B45:G54">
+    <filterColumn colId="0" hiddenButton="1"/>
+    <filterColumn colId="1" hiddenButton="1"/>
+    <filterColumn colId="2" hiddenButton="1"/>
+    <filterColumn colId="3" hiddenButton="1"/>
+    <filterColumn colId="4" hiddenButton="1"/>
+    <filterColumn colId="5" hiddenButton="1"/>
+  </autoFilter>
   <tableColumns count="6">
     <tableColumn id="1" name="Story points " totalsRowLabel="Total" dataDxfId="193" totalsRowDxfId="192"/>
     <tableColumn id="2" name="Min." dataDxfId="191" totalsRowDxfId="190"/>
@@ -4775,9 +3388,9 @@
 </table>
 </file>
 
-<file path=xl/tables/table7.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="Tabla181011234" displayName="Tabla181011234" ref="B87:G96" headerRowDxfId="181" headerRowBorderDxfId="180">
-  <autoFilter ref="B87:G96"/>
+<file path=xl/tables/table5.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Tabla1810112" displayName="Tabla1810112" ref="B59:G68" headerRowDxfId="181" headerRowBorderDxfId="180">
+  <autoFilter ref="B59:G68"/>
   <tableColumns count="6">
     <tableColumn id="1" name="Story points " totalsRowLabel="Total" dataDxfId="179" totalsRowDxfId="178"/>
     <tableColumn id="2" name="Min." dataDxfId="177" totalsRowDxfId="176"/>
@@ -4790,9 +3403,9 @@
 </table>
 </file>
 
-<file path=xl/tables/table8.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="4" name="Tabla1810112345" displayName="Tabla1810112345" ref="B101:G110" headerRowDxfId="167" headerRowBorderDxfId="166">
-  <autoFilter ref="B101:G110"/>
+<file path=xl/tables/table6.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Tabla18101123" displayName="Tabla18101123" ref="B73:G82" headerRowDxfId="167" headerRowBorderDxfId="166">
+  <autoFilter ref="B73:G82"/>
   <tableColumns count="6">
     <tableColumn id="1" name="Story points " totalsRowLabel="Total" dataDxfId="165" totalsRowDxfId="164"/>
     <tableColumn id="2" name="Min." dataDxfId="163" totalsRowDxfId="162"/>
@@ -4805,9 +3418,9 @@
 </table>
 </file>
 
-<file path=xl/tables/table9.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="5" name="Tabla18101123456" displayName="Tabla18101123456" ref="B115:G124" headerRowDxfId="153" headerRowBorderDxfId="152">
-  <autoFilter ref="B115:G124"/>
+<file path=xl/tables/table7.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="Tabla181011234" displayName="Tabla181011234" ref="B87:G96" headerRowDxfId="153" headerRowBorderDxfId="152">
+  <autoFilter ref="B87:G96"/>
   <tableColumns count="6">
     <tableColumn id="1" name="Story points " totalsRowLabel="Total" dataDxfId="151" totalsRowDxfId="150"/>
     <tableColumn id="2" name="Min." dataDxfId="149" totalsRowDxfId="148"/>
@@ -4815,6 +3428,36 @@
     <tableColumn id="4" name="Total" dataDxfId="145" totalsRowDxfId="144"/>
     <tableColumn id="5" name="Real" dataDxfId="143" totalsRowDxfId="142"/>
     <tableColumn id="6" name="Total3" totalsRowFunction="sum" dataDxfId="141" totalsRowDxfId="140"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium16" showFirstColumn="0" showLastColumn="0" showRowStripes="0" showColumnStripes="1"/>
+</table>
+</file>
+
+<file path=xl/tables/table8.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="4" name="Tabla1810112345" displayName="Tabla1810112345" ref="B101:G110" headerRowDxfId="139" headerRowBorderDxfId="138">
+  <autoFilter ref="B101:G110"/>
+  <tableColumns count="6">
+    <tableColumn id="1" name="Story points " totalsRowLabel="Total" dataDxfId="137" totalsRowDxfId="136"/>
+    <tableColumn id="2" name="Min." dataDxfId="135" totalsRowDxfId="134"/>
+    <tableColumn id="3" name="Estimado" dataDxfId="133" totalsRowDxfId="132"/>
+    <tableColumn id="4" name="Total" dataDxfId="131" totalsRowDxfId="130"/>
+    <tableColumn id="5" name="Real" dataDxfId="129" totalsRowDxfId="128"/>
+    <tableColumn id="6" name="Total3" totalsRowFunction="sum" dataDxfId="127" totalsRowDxfId="126"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium16" showFirstColumn="0" showLastColumn="0" showRowStripes="0" showColumnStripes="1"/>
+</table>
+</file>
+
+<file path=xl/tables/table9.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="5" name="Tabla18101123456" displayName="Tabla18101123456" ref="B115:G124" headerRowDxfId="125" headerRowBorderDxfId="124">
+  <autoFilter ref="B115:G124"/>
+  <tableColumns count="6">
+    <tableColumn id="1" name="Story points " totalsRowLabel="Total" dataDxfId="123" totalsRowDxfId="122"/>
+    <tableColumn id="2" name="Min." dataDxfId="121" totalsRowDxfId="120"/>
+    <tableColumn id="3" name="Estimado" dataDxfId="119" totalsRowDxfId="118"/>
+    <tableColumn id="4" name="Total" dataDxfId="117" totalsRowDxfId="116"/>
+    <tableColumn id="5" name="Real" dataDxfId="115" totalsRowDxfId="114"/>
+    <tableColumn id="6" name="Total3" totalsRowFunction="sum" dataDxfId="113" totalsRowDxfId="112"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium16" showFirstColumn="0" showLastColumn="0" showRowStripes="0" showColumnStripes="1"/>
 </table>
@@ -5117,10 +3760,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B1:L273"/>
+  <dimension ref="B1:J236"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B263" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="F269" sqref="F269"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="J4" sqref="J4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5172,8 +3815,8 @@
         <v>23</v>
       </c>
       <c r="J3" s="25">
-        <f>E12+E26+E40+E54+E68+E82+E96+E110+E124+E138+E152+E166+E180+E194+E208+E222+E236+E250+E264</f>
-        <v>661.75</v>
+        <f>E12+E26+E40+E54+E68+E82+E96+E110+E124+E138+E152+E166+E180+E194+E208+E222+E236</f>
+        <v>567.25</v>
       </c>
     </row>
     <row r="4" spans="2:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -5201,8 +3844,8 @@
         <v>24</v>
       </c>
       <c r="J4" s="25">
-        <f>G12+G40+G54+G68+G82+G96+G110+G124+G138+G152+G166+G180+G194+G208+G222+G236+G250+G264</f>
-        <v>794.5</v>
+        <f>G12+G40+G54+G68+G82+G96+G110+G124+G138+G152+G166+G180+G194+G208+G222+G236</f>
+        <v>697</v>
       </c>
     </row>
     <row r="5" spans="2:10" x14ac:dyDescent="0.25">
@@ -9129,707 +7772,13 @@
         <v>45.25</v>
       </c>
     </row>
-    <row r="239" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B239" s="26" t="s">
-        <v>26</v>
-      </c>
-      <c r="C239" s="26"/>
-      <c r="D239" s="26"/>
-      <c r="E239" s="26"/>
-      <c r="F239" s="26"/>
-      <c r="G239" s="26"/>
-    </row>
-    <row r="240" spans="2:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B240" s="27"/>
-      <c r="C240" s="27"/>
-      <c r="D240" s="27"/>
-      <c r="E240" s="27"/>
-      <c r="F240" s="27"/>
-      <c r="G240" s="27"/>
-    </row>
-    <row r="241" spans="2:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B241" s="5" t="s">
-        <v>0</v>
-      </c>
-      <c r="C241" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="D241" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="E241" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="F241" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="G241" s="8" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="242" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B242" s="14">
-        <v>1</v>
-      </c>
-      <c r="C242" s="8">
-        <v>15</v>
-      </c>
-      <c r="D242" s="7">
-        <v>0</v>
-      </c>
-      <c r="E242" s="8">
-        <f>D242*C242</f>
-        <v>0</v>
-      </c>
-      <c r="F242" s="11">
-        <v>0</v>
-      </c>
-      <c r="G242" s="18">
-        <f>F242*C242</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="243" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B243" s="15">
-        <v>2</v>
-      </c>
-      <c r="C243" s="10">
-        <v>45</v>
-      </c>
-      <c r="D243" s="9">
-        <v>2</v>
-      </c>
-      <c r="E243" s="10">
-        <f t="shared" ref="E243:E249" si="34">D243*C243</f>
-        <v>90</v>
-      </c>
-      <c r="F243" s="12">
-        <v>2</v>
-      </c>
-      <c r="G243" s="19">
-        <f t="shared" ref="G243:G249" si="35">F243*C243</f>
-        <v>90</v>
-      </c>
-    </row>
-    <row r="244" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B244" s="15">
-        <v>3</v>
-      </c>
-      <c r="C244" s="10">
-        <v>120</v>
-      </c>
-      <c r="D244" s="9">
-        <v>3</v>
-      </c>
-      <c r="E244" s="10">
-        <f t="shared" si="34"/>
-        <v>360</v>
-      </c>
-      <c r="F244" s="12">
-        <v>2</v>
-      </c>
-      <c r="G244" s="19">
-        <f t="shared" si="35"/>
-        <v>240</v>
-      </c>
-    </row>
-    <row r="245" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B245" s="15">
-        <v>5</v>
-      </c>
-      <c r="C245" s="10">
-        <v>300</v>
-      </c>
-      <c r="D245" s="9">
-        <v>2</v>
-      </c>
-      <c r="E245" s="10">
-        <f t="shared" si="34"/>
-        <v>600</v>
-      </c>
-      <c r="F245" s="12">
-        <v>3</v>
-      </c>
-      <c r="G245" s="19">
-        <f t="shared" si="35"/>
-        <v>900</v>
-      </c>
-    </row>
-    <row r="246" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B246" s="15">
-        <v>8</v>
-      </c>
-      <c r="C246" s="10">
-        <v>720</v>
-      </c>
-      <c r="D246" s="9">
-        <v>1</v>
-      </c>
-      <c r="E246" s="10">
-        <f t="shared" si="34"/>
-        <v>720</v>
-      </c>
-      <c r="F246" s="12">
-        <v>1</v>
-      </c>
-      <c r="G246" s="19">
-        <f t="shared" si="35"/>
-        <v>720</v>
-      </c>
-    </row>
-    <row r="247" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B247" s="15">
-        <v>13</v>
-      </c>
-      <c r="C247" s="10">
-        <v>1440</v>
-      </c>
-      <c r="D247" s="9">
-        <v>1</v>
-      </c>
-      <c r="E247" s="10">
-        <f t="shared" si="34"/>
-        <v>1440</v>
-      </c>
-      <c r="F247" s="12">
-        <v>1</v>
-      </c>
-      <c r="G247" s="19">
-        <f t="shared" si="35"/>
-        <v>1440</v>
-      </c>
-    </row>
-    <row r="248" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B248" s="15">
-        <v>21</v>
-      </c>
-      <c r="C248" s="10">
-        <f>2.5*24*60</f>
-        <v>3600</v>
-      </c>
-      <c r="D248" s="9">
-        <v>0</v>
-      </c>
-      <c r="E248" s="10">
-        <f t="shared" si="34"/>
-        <v>0</v>
-      </c>
-      <c r="F248" s="12">
-        <v>0</v>
-      </c>
-      <c r="G248" s="19">
-        <f t="shared" si="35"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="249" spans="2:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B249" s="15">
-        <v>40</v>
-      </c>
-      <c r="C249" s="10">
-        <f>7*24*60</f>
-        <v>10080</v>
-      </c>
-      <c r="D249" s="9">
-        <v>0</v>
-      </c>
-      <c r="E249" s="10">
-        <f t="shared" si="34"/>
-        <v>0</v>
-      </c>
-      <c r="F249" s="12">
-        <v>0</v>
-      </c>
-      <c r="G249" s="20">
-        <f t="shared" si="35"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="250" spans="2:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B250" s="3"/>
-      <c r="C250" s="16"/>
-      <c r="D250" s="6" t="s">
-        <v>3</v>
-      </c>
-      <c r="E250" s="22">
-        <f>SUM(E242:E249)/60</f>
-        <v>53.5</v>
-      </c>
-      <c r="F250" s="13" t="s">
-        <v>3</v>
-      </c>
-      <c r="G250" s="21">
-        <f>SUM(G242:G249)/60</f>
-        <v>56.5</v>
-      </c>
-    </row>
-    <row r="253" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B253" s="26" t="s">
-        <v>27</v>
-      </c>
-      <c r="C253" s="26"/>
-      <c r="D253" s="26"/>
-      <c r="E253" s="26"/>
-      <c r="F253" s="26"/>
-      <c r="G253" s="26"/>
-    </row>
-    <row r="254" spans="2:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B254" s="27"/>
-      <c r="C254" s="27"/>
-      <c r="D254" s="27"/>
-      <c r="E254" s="27"/>
-      <c r="F254" s="27"/>
-      <c r="G254" s="27"/>
-    </row>
-    <row r="255" spans="2:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B255" s="5" t="s">
-        <v>0</v>
-      </c>
-      <c r="C255" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="D255" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="E255" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="F255" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="G255" s="8" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="256" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B256" s="14">
-        <v>1</v>
-      </c>
-      <c r="C256" s="8">
-        <v>15</v>
-      </c>
-      <c r="D256" s="7">
-        <v>0</v>
-      </c>
-      <c r="E256" s="8">
-        <f>D256*C256</f>
-        <v>0</v>
-      </c>
-      <c r="F256" s="11">
-        <v>0</v>
-      </c>
-      <c r="G256" s="18">
-        <f>F256*C256</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="257" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B257" s="15">
-        <v>2</v>
-      </c>
-      <c r="C257" s="10">
-        <v>45</v>
-      </c>
-      <c r="D257" s="9">
-        <v>4</v>
-      </c>
-      <c r="E257" s="10">
-        <f t="shared" ref="E257:E263" si="36">D257*C257</f>
-        <v>180</v>
-      </c>
-      <c r="F257" s="12">
-        <v>4</v>
-      </c>
-      <c r="G257" s="19">
-        <f t="shared" ref="G257:G263" si="37">F257*C257</f>
-        <v>180</v>
-      </c>
-    </row>
-    <row r="258" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B258" s="15">
-        <v>3</v>
-      </c>
-      <c r="C258" s="10">
-        <v>120</v>
-      </c>
-      <c r="D258" s="9">
-        <v>1</v>
-      </c>
-      <c r="E258" s="10">
-        <f t="shared" si="36"/>
-        <v>120</v>
-      </c>
-      <c r="F258" s="12">
-        <v>1</v>
-      </c>
-      <c r="G258" s="19">
-        <f t="shared" si="37"/>
-        <v>120</v>
-      </c>
-    </row>
-    <row r="259" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B259" s="15">
-        <v>5</v>
-      </c>
-      <c r="C259" s="10">
-        <v>300</v>
-      </c>
-      <c r="D259" s="9">
-        <v>0</v>
-      </c>
-      <c r="E259" s="10">
-        <f t="shared" si="36"/>
-        <v>0</v>
-      </c>
-      <c r="F259" s="12">
-        <v>0</v>
-      </c>
-      <c r="G259" s="19">
-        <f t="shared" si="37"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="260" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B260" s="15">
-        <v>8</v>
-      </c>
-      <c r="C260" s="10">
-        <v>720</v>
-      </c>
-      <c r="D260" s="9">
-        <v>1</v>
-      </c>
-      <c r="E260" s="10">
-        <f t="shared" si="36"/>
-        <v>720</v>
-      </c>
-      <c r="F260" s="12">
-        <v>1</v>
-      </c>
-      <c r="G260" s="19">
-        <f t="shared" si="37"/>
-        <v>720</v>
-      </c>
-    </row>
-    <row r="261" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B261" s="15">
-        <v>13</v>
-      </c>
-      <c r="C261" s="10">
-        <v>1440</v>
-      </c>
-      <c r="D261" s="9">
-        <v>1</v>
-      </c>
-      <c r="E261" s="10">
-        <f t="shared" si="36"/>
-        <v>1440</v>
-      </c>
-      <c r="F261" s="12">
-        <v>1</v>
-      </c>
-      <c r="G261" s="19">
-        <f t="shared" si="37"/>
-        <v>1440</v>
-      </c>
-    </row>
-    <row r="262" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B262" s="15">
-        <v>21</v>
-      </c>
-      <c r="C262" s="10">
-        <f>2.5*24*60</f>
-        <v>3600</v>
-      </c>
-      <c r="D262" s="9">
-        <v>0</v>
-      </c>
-      <c r="E262" s="10">
-        <f t="shared" si="36"/>
-        <v>0</v>
-      </c>
-      <c r="F262" s="12">
-        <v>0</v>
-      </c>
-      <c r="G262" s="19">
-        <f t="shared" si="37"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="263" spans="2:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B263" s="15">
-        <v>40</v>
-      </c>
-      <c r="C263" s="10">
-        <f>7*24*60</f>
-        <v>10080</v>
-      </c>
-      <c r="D263" s="9">
-        <v>0</v>
-      </c>
-      <c r="E263" s="10">
-        <f t="shared" si="36"/>
-        <v>0</v>
-      </c>
-      <c r="F263" s="12">
-        <v>0</v>
-      </c>
-      <c r="G263" s="20">
-        <f t="shared" si="37"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="264" spans="2:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B264" s="3"/>
-      <c r="C264" s="16"/>
-      <c r="D264" s="6" t="s">
-        <v>3</v>
-      </c>
-      <c r="E264" s="22">
-        <f>SUM(E256:E263)/60</f>
-        <v>41</v>
-      </c>
-      <c r="F264" s="13" t="s">
-        <v>3</v>
-      </c>
-      <c r="G264" s="21">
-        <f>SUM(G256:G263)/60</f>
-        <v>41</v>
-      </c>
-    </row>
-    <row r="267" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="C267" t="s">
-        <v>29</v>
-      </c>
-      <c r="D267">
-        <v>1</v>
-      </c>
-      <c r="E267">
-        <v>2</v>
-      </c>
-      <c r="F267">
-        <v>3</v>
-      </c>
-      <c r="G267">
-        <v>5</v>
-      </c>
-      <c r="H267">
-        <v>8</v>
-      </c>
-      <c r="I267">
-        <v>13</v>
-      </c>
-      <c r="J267">
-        <v>21</v>
-      </c>
-      <c r="K267" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="268" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B268" t="s">
-        <v>28</v>
-      </c>
-      <c r="C268">
-        <v>26</v>
-      </c>
-      <c r="D268">
-        <v>3</v>
-      </c>
-      <c r="E268">
-        <v>16</v>
-      </c>
-      <c r="F268">
-        <v>3</v>
-      </c>
-      <c r="G268">
-        <v>2</v>
-      </c>
-      <c r="H268">
-        <v>1</v>
-      </c>
-      <c r="I268">
-        <v>0</v>
-      </c>
-      <c r="J268">
-        <v>0</v>
-      </c>
-      <c r="K268" s="28">
-        <f>(D268*15+E268*45+F268*120+G268*300+H268*720+I268*1440+J268*3600)/60</f>
-        <v>40.75</v>
-      </c>
-      <c r="L268" s="29">
-        <f>K268/$K$273</f>
-        <v>5.1322418136020148E-2</v>
-      </c>
-    </row>
-    <row r="269" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B269" t="s">
-        <v>31</v>
-      </c>
-      <c r="C269">
-        <v>41</v>
-      </c>
-      <c r="D269">
-        <v>11</v>
-      </c>
-      <c r="E269">
-        <v>7</v>
-      </c>
-      <c r="F269">
-        <v>10</v>
-      </c>
-      <c r="G269">
-        <v>6</v>
-      </c>
-      <c r="H269">
-        <v>5</v>
-      </c>
-      <c r="I269">
-        <v>2</v>
-      </c>
-      <c r="J269">
-        <v>0</v>
-      </c>
-      <c r="K269" s="28">
-        <f t="shared" ref="K269:K272" si="38">(D269*15+E269*45+F269*120+G269*300+H269*720+I269*1440+J269*3600)/60</f>
-        <v>166</v>
-      </c>
-      <c r="L269" s="29">
-        <f t="shared" ref="L269:L272" si="39">K269/$K$273</f>
-        <v>0.20906801007556675</v>
-      </c>
-    </row>
-    <row r="270" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B270" t="s">
-        <v>32</v>
-      </c>
-      <c r="C270">
-        <v>63</v>
-      </c>
-      <c r="D270">
-        <v>3</v>
-      </c>
-      <c r="E270">
-        <v>14</v>
-      </c>
-      <c r="F270">
-        <v>12</v>
-      </c>
-      <c r="G270">
-        <v>15</v>
-      </c>
-      <c r="H270">
-        <v>16</v>
-      </c>
-      <c r="I270">
-        <v>2</v>
-      </c>
-      <c r="J270">
-        <v>1</v>
-      </c>
-      <c r="K270" s="28">
-        <f t="shared" si="38"/>
-        <v>410.25</v>
-      </c>
-      <c r="L270" s="29">
-        <f t="shared" si="39"/>
-        <v>0.51668765743073053</v>
-      </c>
-    </row>
-    <row r="271" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B271" t="s">
-        <v>33</v>
-      </c>
-      <c r="C271">
-        <v>30</v>
-      </c>
-      <c r="D271">
-        <v>0</v>
-      </c>
-      <c r="E271">
-        <v>8</v>
-      </c>
-      <c r="F271">
-        <v>10</v>
-      </c>
-      <c r="G271">
-        <v>6</v>
-      </c>
-      <c r="H271">
-        <v>6</v>
-      </c>
-      <c r="I271">
-        <v>0</v>
-      </c>
-      <c r="J271">
-        <v>0</v>
-      </c>
-      <c r="K271" s="28">
-        <f t="shared" si="38"/>
-        <v>128</v>
-      </c>
-      <c r="L271" s="29">
-        <f t="shared" si="39"/>
-        <v>0.16120906801007556</v>
-      </c>
-    </row>
-    <row r="272" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B272" t="s">
-        <v>34</v>
-      </c>
-      <c r="C272">
-        <v>7</v>
-      </c>
-      <c r="D272">
-        <v>0</v>
-      </c>
-      <c r="E272">
-        <v>0</v>
-      </c>
-      <c r="F272">
-        <v>4</v>
-      </c>
-      <c r="G272">
-        <v>1</v>
-      </c>
-      <c r="H272">
-        <v>1</v>
-      </c>
-      <c r="I272">
-        <v>1</v>
-      </c>
-      <c r="J272">
-        <v>0</v>
-      </c>
-      <c r="K272" s="28">
-        <f t="shared" si="38"/>
-        <v>49</v>
-      </c>
-      <c r="L272" s="29">
-        <f t="shared" si="39"/>
-        <v>6.1712846347607056E-2</v>
-      </c>
-    </row>
-    <row r="273" spans="3:11" x14ac:dyDescent="0.25">
-      <c r="C273">
-        <f>SUM(C268:C272)</f>
-        <v>167</v>
-      </c>
-      <c r="K273" s="28">
-        <f>SUM(K268:K272)</f>
-        <v>794</v>
-      </c>
-    </row>
   </sheetData>
-  <mergeCells count="19">
-    <mergeCell ref="B239:G240"/>
-    <mergeCell ref="B253:G254"/>
-    <mergeCell ref="B1:G2"/>
-    <mergeCell ref="B15:G16"/>
-    <mergeCell ref="B29:G30"/>
-    <mergeCell ref="B43:G44"/>
-    <mergeCell ref="B57:G58"/>
+  <mergeCells count="17">
+    <mergeCell ref="B225:G226"/>
+    <mergeCell ref="B211:G212"/>
+    <mergeCell ref="B127:G128"/>
+    <mergeCell ref="B113:G114"/>
+    <mergeCell ref="B99:G100"/>
     <mergeCell ref="B71:G72"/>
     <mergeCell ref="B85:G86"/>
     <mergeCell ref="B197:G198"/>
@@ -9837,16 +7786,16 @@
     <mergeCell ref="B169:G170"/>
     <mergeCell ref="B155:G156"/>
     <mergeCell ref="B141:G142"/>
-    <mergeCell ref="B225:G226"/>
-    <mergeCell ref="B211:G212"/>
-    <mergeCell ref="B127:G128"/>
-    <mergeCell ref="B113:G114"/>
-    <mergeCell ref="B99:G100"/>
+    <mergeCell ref="B1:G2"/>
+    <mergeCell ref="B15:G16"/>
+    <mergeCell ref="B29:G30"/>
+    <mergeCell ref="B43:G44"/>
+    <mergeCell ref="B57:G58"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
-  <drawing r:id="rId2"/>
-  <tableParts count="19">
+  <tableParts count="17">
+    <tablePart r:id="rId2"/>
     <tablePart r:id="rId3"/>
     <tablePart r:id="rId4"/>
     <tablePart r:id="rId5"/>
@@ -9863,9 +7812,6 @@
     <tablePart r:id="rId16"/>
     <tablePart r:id="rId17"/>
     <tablePart r:id="rId18"/>
-    <tablePart r:id="rId19"/>
-    <tablePart r:id="rId20"/>
-    <tablePart r:id="rId21"/>
   </tableParts>
 </worksheet>
 </file>
</xml_diff>